<commit_message>
categories (groups and keywords) in handle_obvious_dups
</commit_message>
<xml_diff>
--- a/inst/extdata/3dupsin5refs.xlsx
+++ b/inst/extdata/3dupsin5refs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://biomathgmbh.sharepoint.com/sites/bm/Freigegebene Dokumente/BM Tools/R/CitaviR/CitaviR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_3D259F2FE6F535567F541EDB38B72A6C57C387C5" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A67A4DEC-457F-4BE4-8694-AA9F60D75D28}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_3D259F2FE6F535567F541EDB38B72A6C57C387C5" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{08C44687-648C-4EF7-B814-710D0E0D283C}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>Author</t>
   </si>
@@ -200,6 +200,12 @@
   </si>
   <si>
     <t>DOI name</t>
+  </si>
+  <si>
+    <t>1 catA</t>
+  </si>
+  <si>
+    <t>2 catB</t>
   </si>
 </sst>
 </file>
@@ -682,9 +688,7 @@
   </sheetPr>
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -796,7 +800,7 @@
         <v>26</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>33</v>
@@ -858,7 +862,7 @@
         <v>26</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>33</v>
@@ -918,7 +922,7 @@
         <v>26</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>23</v>
@@ -980,7 +984,7 @@
         <v>26</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>15</v>
@@ -1042,7 +1046,7 @@
         <v>10</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>33</v>
@@ -1081,12 +1085,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1268,15 +1269,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8396E0C8-24DD-4AFF-B903-A0BEFC2FAAF4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6B7FE0F-3381-4F74-A10B-D234BF05433F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1300,10 +1305,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6B7FE0F-3381-4F74-A10B-D234BF05433F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8396E0C8-24DD-4AFF-B903-A0BEFC2FAAF4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>